<commit_message>
Update DateBase/orders/International Ever Green_2025-11-7.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/International Ever Green_2025-11-7.xlsx
+++ b/DateBase/orders/International Ever Green_2025-11-7.xlsx
@@ -702,6 +702,9 @@
       <c r="C31" t="str">
         <v>106_绣球单瓣粉_Hydrangea Pink S_Hydrangea L._1stem</v>
       </c>
+      <c r="F31" t="str">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -763,7 +766,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>020202627135015131514207562536101034103520142083020850</v>
+        <v>0202026271350151315142075625361010341035201420830208540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>